<commit_message>
Changed airfoil path from Default to NACA_0012
</commit_message>
<xml_diff>
--- a/Input/Files/input.xlsx
+++ b/Input/Files/input.xlsx
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Fuselage</t>
   </si>
   <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t>Geometry</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>deg</t>
   </si>
   <si>
-    <t>wing</t>
-  </si>
-  <si>
     <t>aspectRatio</t>
   </si>
   <si>
@@ -83,6 +74,12 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>EOF</t>
+  </si>
+  <si>
+    <t>Wing</t>
   </si>
 </sst>
 </file>
@@ -462,159 +459,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="D7"/>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12"/>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13"/>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15"/>
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
+      <c r="C16" s="1"/>
+      <c r="D16"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="D35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finalized the excel importer
</commit_message>
<xml_diff>
--- a/Input/Files/input.xlsx
+++ b/Input/Files/input.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
merge ExampleWing and Wing
</commit_message>
<xml_diff>
--- a/Input/Files/input.xlsx
+++ b/Input/Files/input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>EOC</t>
   </si>
   <si>
-    <t>Aircraft</t>
-  </si>
-  <si>
     <t>M cruise</t>
   </si>
   <si>
@@ -137,12 +134,15 @@
   </si>
   <si>
     <t>wing</t>
+  </si>
+  <si>
+    <t>Performance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -180,7 +180,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -271,6 +271,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -306,6 +323,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,25 +518,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -525,14 +559,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>24</v>
       </c>
       <c r="C4">
         <v>0.77</v>
@@ -541,19 +575,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -567,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -581,7 +615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -593,7 +627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -605,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -619,23 +653,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -645,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -655,7 +689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -665,27 +699,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -695,51 +729,51 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1">
         <v>340.3</v>
       </c>
       <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>28</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>29</v>
       </c>
       <c r="C25" s="1">
         <v>1.2250000000000001</v>
       </c>
       <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>31</v>
       </c>
       <c r="C26" s="1">
         <v>1375</v>
       </c>
       <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>32</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>33</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -749,9 +783,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1">
         <v>0.97</v>
@@ -761,9 +795,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1">
         <v>0.75</v>
@@ -773,21 +807,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1">
         <v>0.75</v>
@@ -797,34 +831,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36"/>
     </row>

</xml_diff>

<commit_message>
Sistemazione engine position e wing position
</commit_message>
<xml_diff>
--- a/Input/Files/input.xlsx
+++ b/Input/Files/input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Fuselage</t>
   </si>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,13 +844,16 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>20</v>
+      <c r="B33" t="s">
+        <v>22</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34"/>
     </row>

</xml_diff>